<commit_message>
scores by school spending.
</commit_message>
<xml_diff>
--- a/Resources/pandas_cheat_sheet.xlsx
+++ b/Resources/pandas_cheat_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcort\bootcamp\School_District_Analysis\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B8E62B-50E6-429C-AD5C-898C7D8E4E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F51494A-B1B2-422C-B8FE-A0EF02C23306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46455" yWindow="-90" windowWidth="11025" windowHeight="15690" activeTab="1" xr2:uid="{E67E81BA-80AC-42E9-9E5C-A9A2309DB558}"/>
+    <workbookView xWindow="17655" yWindow="0" windowWidth="11025" windowHeight="15600" activeTab="1" xr2:uid="{E67E81BA-80AC-42E9-9E5C-A9A2309DB558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1168,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB5665F-799D-49FD-8954-67C9C00235B5}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,42 +1629,42 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="17" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="17" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="17" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1723,14 +1733,19 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B50:B1048576 B1:B47">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Commit Your Code">
+  <conditionalFormatting sqref="B50:B55 B1:B47 B61:B1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Commit Your Code">
       <formula>NOT(ISERROR(SEARCH("Commit Your Code",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B49">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Commit Your Code">
+      <formula>NOT(ISERROR(SEARCH("Commit Your Code",B48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Commit Your Code">
-      <formula>NOT(ISERROR(SEARCH("Commit Your Code",B48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Commit Your Code",B60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>